<commit_message>
added bci centroid file for board assembly for screaming circuits
</commit_message>
<xml_diff>
--- a/Hardware Files/Schematics and Layout/bcimodule/BOM BCI Module_Screaming_Circuits.xlsx
+++ b/Hardware Files/Schematics and Layout/bcimodule/BOM BCI Module_Screaming_Circuits.xlsx
@@ -364,7 +364,8 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <charset val="238"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -386,10 +387,10 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
@@ -460,7 +461,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -483,21 +484,21 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
@@ -518,26 +519,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
-      <selection activeCell="C26" activeCellId="0" pane="topLeft" sqref="C26"/>
+      <selection activeCell="D27" activeCellId="0" pane="topLeft" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.58823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.5294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="30.9294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.8392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="45.9019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.2313725490196"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="45.9019607843137"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="29.8392156862745"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.5294117647059"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.4980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.6274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="31.0588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.9607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="46.0941176470588"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.9176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.3176470588235"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="46.0941176470588"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="29.9607843137255"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.6274509803922"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.5686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.22352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1" s="3">
@@ -568,10 +569,6 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="4" t="n">
@@ -776,71 +773,63 @@
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9" s="9">
-      <c r="A9" s="8" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9" s="1">
+      <c r="A9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="0"/>
-      <c r="K9" s="0"/>
-      <c r="L9" s="0"/>
-      <c r="M9" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10" s="9">
-      <c r="A10" s="8" t="n">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10" s="1">
+      <c r="A10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="0"/>
-      <c r="K10" s="0"/>
-      <c r="L10" s="0"/>
-      <c r="M10" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="4" t="n">
@@ -871,63 +860,55 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12" s="9">
-      <c r="A12" s="8" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12" s="1">
+      <c r="A12" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="0"/>
-      <c r="K12" s="0"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13" s="9">
-      <c r="A13" s="8" t="n">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13" s="1">
+      <c r="A13" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="0"/>
-      <c r="K13" s="0"/>
-      <c r="L13" s="0"/>
-      <c r="M13" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="4" t="n">
@@ -959,58 +940,46 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="H17" s="0"/>
-      <c r="I17" s="0"/>
+      <c r="E17" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="13" t="n">
+      <c r="E18" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="13" t="n">
+      <c r="E19" s="11" t="n">
         <v>42</v>
       </c>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="H20" s="0"/>
-      <c r="I20" s="0"/>
+      <c r="E20" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="13" t="n">
+      <c r="E21" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="H21" s="0"/>
-      <c r="I21" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="H22" s="0"/>
-      <c r="I22" s="0"/>
+      <c r="E22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1038,7 +1007,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1063,7 +1032,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>